<commit_message>
pancr fix pancreatic vasculature to wbkg pancreatic acinus
</commit_message>
<xml_diff>
--- a/models/pancreas/source/pancreas.xlsx
+++ b/models/pancreas/source/pancreas.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="417">
   <si>
     <t>id</t>
   </si>
@@ -936,7 +936,7 @@
     <t>0,3,0</t>
   </si>
   <si>
-    <t>wbkg:lyph-PNS-ganglion-intrapancreatic,lyph-pancreatic-vasculature,wbkg:lyph-pancreatic-islet-of-langerhans</t>
+    <t>wbkg:lyph-PNS-ganglion-intrapancreatic,wbkg:lyph-pancreatic-acinus,wbkg:lyph-pancreatic-islet-of-langerhans</t>
   </si>
   <si>
     <t>dendrite-chain-interpancreatic-ganglia-islets-neuron-3</t>
@@ -955,9 +955,6 @@
   </si>
   <si>
     <t>con_isle3</t>
-  </si>
-  <si>
-    <t>wbkg:lyph-PNS-ganglion-intrapancreatic,wbkg:lyph-pancreatic-acinus,wbkg:lyph-pancreatic-islet-of-langerhans</t>
   </si>
   <si>
     <t>dendrite-chain-proximal-duodenum-neuron-4</t>
@@ -1638,7 +1635,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="209">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2035,6 +2032,9 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -2044,6 +2044,9 @@
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="19" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -2057,6 +2060,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="19" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2073,6 +2079,9 @@
     </xf>
     <xf borderId="0" fillId="20" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="20" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="20" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -2095,6 +2104,9 @@
     </xf>
     <xf borderId="0" fillId="20" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -2567,50 +2579,50 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="193" t="s">
+      <c r="B1" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="193" t="s">
+      <c r="D1" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="193" t="s">
+      <c r="E1" s="198" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="193" t="s">
-        <v>378</v>
+      <c r="F1" s="198" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="200" t="s">
         <v>381</v>
-      </c>
-      <c r="E2" s="195" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="74" t="s">
-        <v>385</v>
-      </c>
-      <c r="E3" s="195" t="s">
-        <v>382</v>
+        <v>384</v>
+      </c>
+      <c r="E3" s="200" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -2634,18 +2646,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="196" t="s">
-        <v>386</v>
+      <c r="A1" s="201" t="s">
+        <v>385</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="197"/>
+      <c r="A2" s="202"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2667,130 +2679,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="198" t="s">
+      <c r="A2" s="203" t="s">
+        <v>388</v>
+      </c>
+      <c r="B2" s="204" t="s">
         <v>389</v>
       </c>
-      <c r="B2" s="199" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="203" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="198" t="s">
+      <c r="B3" s="205" t="s">
         <v>391</v>
       </c>
-      <c r="B3" s="200" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="203" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="198" t="s">
+      <c r="B4" s="206" t="s">
         <v>393</v>
       </c>
-      <c r="B4" s="201" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="203" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="198" t="s">
+      <c r="B5" s="206" t="s">
         <v>395</v>
       </c>
-      <c r="B5" s="201" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="203" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="198" t="s">
+      <c r="B6" s="206" t="s">
         <v>397</v>
       </c>
-      <c r="B6" s="201" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="203" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="198" t="s">
+      <c r="B7" s="206" t="s">
         <v>399</v>
       </c>
-      <c r="B7" s="201" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="203" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="198" t="s">
+      <c r="B8" s="206" t="s">
         <v>401</v>
       </c>
-      <c r="B8" s="201" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="203" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="198" t="s">
+      <c r="B9" s="206" t="s">
         <v>403</v>
       </c>
-      <c r="B9" s="201" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="203" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="198" t="s">
+      <c r="B10" s="206" t="s">
         <v>405</v>
       </c>
-      <c r="B10" s="201" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="203" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="198" t="s">
+      <c r="B11" s="206" t="s">
         <v>407</v>
-      </c>
-      <c r="B11" s="201" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B12" s="197" t="s">
         <v>409</v>
-      </c>
-      <c r="B12" s="192" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="56" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="207" t="s">
         <v>411</v>
-      </c>
-      <c r="B13" s="202" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="203" t="s">
-        <v>413</v>
+      <c r="B14" s="208" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="B15" s="207" t="s">
         <v>414</v>
-      </c>
-      <c r="B15" s="202" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="B16" s="207" t="s">
         <v>416</v>
-      </c>
-      <c r="B16" s="202" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -4793,7 +4805,7 @@
       <c r="A27" s="64" t="s">
         <v>253</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="119" t="s">
         <v>254</v>
       </c>
       <c r="C27" s="102" t="s">
@@ -4829,10 +4841,10 @@
       <c r="A28" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="136" t="s">
         <v>257</v>
       </c>
-      <c r="C28" s="136" t="s">
+      <c r="C28" s="137" t="s">
         <v>198</v>
       </c>
       <c r="D28" s="26"/>
@@ -4842,10 +4854,10 @@
       <c r="F28" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G28" s="137" t="s">
+      <c r="G28" s="138" t="s">
         <v>258</v>
       </c>
-      <c r="H28" s="138"/>
+      <c r="H28" s="139"/>
       <c r="I28" s="54"/>
       <c r="J28" s="54"/>
       <c r="K28" s="121">
@@ -4866,10 +4878,10 @@
       <c r="A29" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="136" t="s">
         <v>261</v>
       </c>
-      <c r="C29" s="136" t="s">
+      <c r="C29" s="137" t="s">
         <v>193</v>
       </c>
       <c r="D29" s="26"/>
@@ -4903,10 +4915,10 @@
       <c r="A30" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="136" t="s">
         <v>264</v>
       </c>
-      <c r="C30" s="136" t="s">
+      <c r="C30" s="137" t="s">
         <v>198</v>
       </c>
       <c r="D30" s="26"/>
@@ -4916,7 +4928,7 @@
       <c r="F30" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G30" s="137" t="s">
+      <c r="G30" s="138" t="s">
         <v>258</v>
       </c>
       <c r="H30" s="16"/>
@@ -4940,32 +4952,32 @@
       <c r="A31" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="140" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="137" t="s">
         <v>198</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="F31" s="137" t="s">
+      <c r="F31" s="138" t="s">
         <v>258</v>
       </c>
-      <c r="G31" s="139" t="s">
+      <c r="G31" s="141" t="s">
         <v>267</v>
       </c>
-      <c r="H31" s="138"/>
+      <c r="H31" s="139"/>
       <c r="I31" s="54"/>
       <c r="J31" s="54"/>
       <c r="K31" s="121" t="s">
         <v>268</v>
       </c>
-      <c r="L31" s="140" t="s">
+      <c r="L31" s="142" t="s">
         <v>269</v>
       </c>
-      <c r="M31" s="141"/>
+      <c r="M31" s="143"/>
       <c r="N31" s="54"/>
       <c r="O31" s="16"/>
       <c r="P31" s="95"/>
@@ -4977,29 +4989,29 @@
       <c r="A32" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="140" t="s">
         <v>271</v>
       </c>
-      <c r="C32" s="136" t="s">
+      <c r="C32" s="137" t="s">
         <v>198</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="F32" s="137" t="s">
+      <c r="F32" s="138" t="s">
         <v>258</v>
       </c>
-      <c r="G32" s="139" t="s">
+      <c r="G32" s="141" t="s">
         <v>267</v>
       </c>
-      <c r="H32" s="138"/>
+      <c r="H32" s="139"/>
       <c r="I32" s="54"/>
       <c r="J32" s="54"/>
       <c r="K32" s="121" t="s">
         <v>268</v>
       </c>
-      <c r="L32" s="140" t="s">
+      <c r="L32" s="142" t="s">
         <v>272</v>
       </c>
       <c r="M32" s="54"/>
@@ -5014,29 +5026,29 @@
       <c r="A33" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="140" t="s">
         <v>274</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="137" t="s">
         <v>198</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="F33" s="137" t="s">
+      <c r="F33" s="138" t="s">
         <v>258</v>
       </c>
-      <c r="G33" s="139" t="s">
+      <c r="G33" s="141" t="s">
         <v>267</v>
       </c>
-      <c r="H33" s="138"/>
+      <c r="H33" s="139"/>
       <c r="I33" s="54"/>
       <c r="J33" s="54"/>
       <c r="K33" s="121" t="s">
         <v>275</v>
       </c>
-      <c r="L33" s="140" t="s">
+      <c r="L33" s="142" t="s">
         <v>276</v>
       </c>
       <c r="M33" s="54"/>
@@ -5048,32 +5060,32 @@
       <c r="S33" s="95"/>
     </row>
     <row r="34">
-      <c r="A34" s="142" t="s">
+      <c r="A34" s="144" t="s">
         <v>277</v>
       </c>
-      <c r="B34" s="142" t="s">
+      <c r="B34" s="145" t="s">
         <v>278</v>
       </c>
       <c r="C34" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="D34" s="143"/>
+      <c r="D34" s="146"/>
       <c r="E34" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="F34" s="144" t="s">
+      <c r="F34" s="147" t="s">
         <v>267</v>
       </c>
-      <c r="G34" s="145" t="s">
+      <c r="G34" s="148" t="s">
         <v>279</v>
       </c>
-      <c r="H34" s="145"/>
+      <c r="H34" s="148"/>
       <c r="I34" s="54"/>
       <c r="J34" s="54"/>
-      <c r="K34" s="146">
+      <c r="K34" s="149">
         <v>0.0</v>
       </c>
-      <c r="L34" s="138" t="s">
+      <c r="L34" s="139" t="s">
         <v>55</v>
       </c>
       <c r="M34" s="54"/>
@@ -5085,32 +5097,32 @@
       <c r="S34" s="54"/>
     </row>
     <row r="35">
-      <c r="A35" s="142" t="s">
+      <c r="A35" s="144" t="s">
         <v>280</v>
       </c>
-      <c r="B35" s="142" t="s">
+      <c r="B35" s="145" t="s">
         <v>281</v>
       </c>
       <c r="C35" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="D35" s="143"/>
+      <c r="D35" s="146"/>
       <c r="E35" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="F35" s="144" t="s">
+      <c r="F35" s="147" t="s">
         <v>267</v>
       </c>
-      <c r="G35" s="145" t="s">
+      <c r="G35" s="148" t="s">
         <v>282</v>
       </c>
-      <c r="H35" s="145"/>
+      <c r="H35" s="148"/>
       <c r="I35" s="54"/>
       <c r="J35" s="54"/>
-      <c r="K35" s="147" t="s">
+      <c r="K35" s="150" t="s">
         <v>283</v>
       </c>
-      <c r="L35" s="138" t="s">
+      <c r="L35" s="21" t="s">
         <v>284</v>
       </c>
       <c r="M35" s="54"/>
@@ -5122,103 +5134,103 @@
       <c r="S35" s="54"/>
     </row>
     <row r="36">
-      <c r="A36" s="148" t="s">
+      <c r="A36" s="151" t="s">
         <v>285</v>
       </c>
-      <c r="B36" s="148" t="s">
+      <c r="B36" s="152" t="s">
         <v>286</v>
       </c>
-      <c r="C36" s="149" t="s">
+      <c r="C36" s="153" t="s">
         <v>193</v>
       </c>
-      <c r="D36" s="150"/>
-      <c r="E36" s="151" t="s">
+      <c r="D36" s="154"/>
+      <c r="E36" s="155" t="s">
         <v>194</v>
       </c>
-      <c r="F36" s="152" t="s">
+      <c r="F36" s="156" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="152" t="s">
+      <c r="G36" s="156" t="s">
         <v>287</v>
       </c>
-      <c r="H36" s="153"/>
-      <c r="I36" s="154"/>
-      <c r="J36" s="154"/>
-      <c r="K36" s="155">
+      <c r="H36" s="157"/>
+      <c r="I36" s="158"/>
+      <c r="J36" s="158"/>
+      <c r="K36" s="159">
         <v>0.0</v>
       </c>
-      <c r="L36" s="148" t="s">
+      <c r="L36" s="151" t="s">
         <v>55</v>
       </c>
-      <c r="M36" s="154"/>
-      <c r="N36" s="154"/>
-      <c r="O36" s="152"/>
-      <c r="P36" s="156"/>
-      <c r="Q36" s="156"/>
-      <c r="R36" s="156"/>
-      <c r="S36" s="156"/>
+      <c r="M36" s="158"/>
+      <c r="N36" s="158"/>
+      <c r="O36" s="156"/>
+      <c r="P36" s="160"/>
+      <c r="Q36" s="160"/>
+      <c r="R36" s="160"/>
+      <c r="S36" s="160"/>
     </row>
     <row r="37">
-      <c r="A37" s="148" t="s">
+      <c r="A37" s="151" t="s">
         <v>288</v>
       </c>
-      <c r="B37" s="148" t="s">
+      <c r="B37" s="152" t="s">
         <v>289</v>
       </c>
-      <c r="C37" s="149" t="s">
+      <c r="C37" s="153" t="s">
         <v>198</v>
       </c>
-      <c r="D37" s="150"/>
-      <c r="E37" s="151" t="s">
+      <c r="D37" s="154"/>
+      <c r="E37" s="155" t="s">
         <v>246</v>
       </c>
-      <c r="F37" s="152" t="s">
+      <c r="F37" s="156" t="s">
         <v>127</v>
       </c>
-      <c r="G37" s="152" t="s">
+      <c r="G37" s="156" t="s">
         <v>290</v>
       </c>
-      <c r="H37" s="153"/>
-      <c r="I37" s="154"/>
-      <c r="J37" s="154"/>
-      <c r="K37" s="155" t="s">
+      <c r="H37" s="157"/>
+      <c r="I37" s="158"/>
+      <c r="J37" s="158"/>
+      <c r="K37" s="159" t="s">
         <v>283</v>
       </c>
-      <c r="L37" s="148" t="s">
-        <v>291</v>
-      </c>
-      <c r="M37" s="154"/>
-      <c r="N37" s="154"/>
-      <c r="O37" s="152"/>
-      <c r="P37" s="156"/>
-      <c r="Q37" s="156"/>
-      <c r="R37" s="156"/>
-      <c r="S37" s="156"/>
+      <c r="L37" s="151" t="s">
+        <v>284</v>
+      </c>
+      <c r="M37" s="158"/>
+      <c r="N37" s="158"/>
+      <c r="O37" s="156"/>
+      <c r="P37" s="160"/>
+      <c r="Q37" s="160"/>
+      <c r="R37" s="160"/>
+      <c r="S37" s="160"/>
     </row>
     <row r="38">
       <c r="A38" s="67" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="161" t="s">
         <v>292</v>
       </c>
-      <c r="B38" s="72" t="s">
-        <v>293</v>
-      </c>
-      <c r="C38" s="157" t="s">
+      <c r="C38" s="162" t="s">
         <v>193</v>
       </c>
-      <c r="D38" s="158"/>
+      <c r="D38" s="163"/>
       <c r="E38" s="73" t="s">
         <v>194</v>
       </c>
       <c r="F38" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="G38" s="159" t="s">
-        <v>294</v>
-      </c>
-      <c r="H38" s="160"/>
+      <c r="G38" s="164" t="s">
+        <v>293</v>
+      </c>
+      <c r="H38" s="165"/>
       <c r="I38" s="70"/>
       <c r="J38" s="70"/>
-      <c r="K38" s="161">
+      <c r="K38" s="166">
         <v>5.0</v>
       </c>
       <c r="L38" s="49" t="s">
@@ -5227,56 +5239,56 @@
       <c r="M38" s="70"/>
       <c r="N38" s="70"/>
       <c r="O38" s="68"/>
-      <c r="P38" s="162"/>
-      <c r="Q38" s="162"/>
-      <c r="R38" s="162"/>
-      <c r="S38" s="162"/>
+      <c r="P38" s="167"/>
+      <c r="Q38" s="167"/>
+      <c r="R38" s="167"/>
+      <c r="S38" s="167"/>
     </row>
     <row r="39">
       <c r="A39" s="67" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" s="161" t="s">
         <v>295</v>
       </c>
-      <c r="B39" s="72" t="s">
-        <v>296</v>
-      </c>
-      <c r="C39" s="157" t="s">
+      <c r="C39" s="162" t="s">
         <v>198</v>
       </c>
-      <c r="D39" s="158"/>
+      <c r="D39" s="163"/>
       <c r="E39" s="73" t="s">
         <v>199</v>
       </c>
       <c r="F39" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="G39" s="159" t="s">
-        <v>297</v>
-      </c>
-      <c r="H39" s="160"/>
+      <c r="G39" s="164" t="s">
+        <v>296</v>
+      </c>
+      <c r="H39" s="165"/>
       <c r="I39" s="70"/>
       <c r="J39" s="70"/>
-      <c r="K39" s="161" t="s">
+      <c r="K39" s="166" t="s">
+        <v>297</v>
+      </c>
+      <c r="L39" s="73" t="s">
         <v>298</v>
-      </c>
-      <c r="L39" s="73" t="s">
-        <v>299</v>
       </c>
       <c r="M39" s="70"/>
       <c r="N39" s="70"/>
       <c r="O39" s="68"/>
-      <c r="P39" s="162"/>
-      <c r="Q39" s="162"/>
-      <c r="R39" s="162"/>
-      <c r="S39" s="162"/>
+      <c r="P39" s="167"/>
+      <c r="Q39" s="167"/>
+      <c r="R39" s="167"/>
+      <c r="S39" s="167"/>
     </row>
     <row r="40">
       <c r="A40" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" s="161" t="s">
         <v>300</v>
       </c>
-      <c r="B40" s="72" t="s">
-        <v>301</v>
-      </c>
-      <c r="C40" s="157" t="s">
+      <c r="C40" s="162" t="s">
         <v>193</v>
       </c>
       <c r="D40" s="70"/>
@@ -5287,10 +5299,10 @@
         <v>134</v>
       </c>
       <c r="G40" s="68" t="s">
-        <v>302</v>
-      </c>
-      <c r="H40" s="163"/>
-      <c r="I40" s="164"/>
+        <v>301</v>
+      </c>
+      <c r="H40" s="168"/>
+      <c r="I40" s="169"/>
       <c r="J40" s="70"/>
       <c r="K40" s="68">
         <v>6.0</v>
@@ -5301,72 +5313,72 @@
       <c r="M40" s="70"/>
       <c r="N40" s="70"/>
       <c r="O40" s="68"/>
-      <c r="P40" s="162"/>
-      <c r="Q40" s="162"/>
-      <c r="R40" s="162"/>
-      <c r="S40" s="162"/>
+      <c r="P40" s="167"/>
+      <c r="Q40" s="167"/>
+      <c r="R40" s="167"/>
+      <c r="S40" s="167"/>
     </row>
     <row r="41">
       <c r="A41" s="67" t="s">
+        <v>302</v>
+      </c>
+      <c r="B41" s="161" t="s">
         <v>303</v>
       </c>
-      <c r="B41" s="72" t="s">
-        <v>304</v>
-      </c>
-      <c r="C41" s="157" t="s">
+      <c r="C41" s="162" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="158"/>
+      <c r="D41" s="163"/>
       <c r="E41" s="73" t="s">
         <v>199</v>
       </c>
       <c r="F41" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="G41" s="159" t="s">
-        <v>297</v>
-      </c>
-      <c r="H41" s="160"/>
+      <c r="G41" s="164" t="s">
+        <v>296</v>
+      </c>
+      <c r="H41" s="165"/>
       <c r="I41" s="70"/>
       <c r="J41" s="70"/>
-      <c r="K41" s="161" t="s">
+      <c r="K41" s="166" t="s">
+        <v>304</v>
+      </c>
+      <c r="L41" s="73" t="s">
         <v>305</v>
-      </c>
-      <c r="L41" s="73" t="s">
-        <v>306</v>
       </c>
       <c r="M41" s="70"/>
       <c r="N41" s="70"/>
       <c r="O41" s="68"/>
-      <c r="P41" s="162"/>
-      <c r="Q41" s="162"/>
-      <c r="R41" s="162"/>
-      <c r="S41" s="162"/>
+      <c r="P41" s="167"/>
+      <c r="Q41" s="167"/>
+      <c r="R41" s="167"/>
+      <c r="S41" s="167"/>
     </row>
     <row r="42">
       <c r="A42" s="67" t="s">
+        <v>306</v>
+      </c>
+      <c r="B42" s="161" t="s">
         <v>307</v>
       </c>
-      <c r="B42" s="72" t="s">
-        <v>308</v>
-      </c>
-      <c r="C42" s="157" t="s">
+      <c r="C42" s="162" t="s">
         <v>198</v>
       </c>
-      <c r="D42" s="158"/>
+      <c r="D42" s="163"/>
       <c r="E42" s="73" t="s">
         <v>246</v>
       </c>
       <c r="F42" s="68" t="s">
-        <v>297</v>
-      </c>
-      <c r="G42" s="159" t="s">
-        <v>309</v>
-      </c>
-      <c r="H42" s="160"/>
+        <v>296</v>
+      </c>
+      <c r="G42" s="164" t="s">
+        <v>308</v>
+      </c>
+      <c r="H42" s="165"/>
       <c r="I42" s="70"/>
       <c r="J42" s="70"/>
-      <c r="K42" s="161">
+      <c r="K42" s="166">
         <v>0.0</v>
       </c>
       <c r="L42" s="135" t="s">
@@ -5375,54 +5387,54 @@
       <c r="M42" s="70"/>
       <c r="N42" s="70"/>
       <c r="O42" s="68"/>
-      <c r="P42" s="162"/>
-      <c r="Q42" s="162"/>
-      <c r="R42" s="162"/>
-      <c r="S42" s="162"/>
+      <c r="P42" s="167"/>
+      <c r="Q42" s="167"/>
+      <c r="R42" s="167"/>
+      <c r="S42" s="167"/>
     </row>
     <row r="43">
       <c r="A43" s="67" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" s="161" t="s">
         <v>310</v>
       </c>
-      <c r="B43" s="72" t="s">
-        <v>311</v>
-      </c>
-      <c r="C43" s="157" t="s">
+      <c r="C43" s="162" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="158"/>
+      <c r="D43" s="163"/>
       <c r="E43" s="73" t="s">
         <v>246</v>
       </c>
       <c r="F43" s="68" t="s">
-        <v>297</v>
-      </c>
-      <c r="G43" s="159" t="s">
-        <v>312</v>
-      </c>
-      <c r="H43" s="160"/>
+        <v>296</v>
+      </c>
+      <c r="G43" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="H43" s="165"/>
       <c r="I43" s="70"/>
       <c r="J43" s="70"/>
-      <c r="K43" s="161" t="s">
+      <c r="K43" s="166" t="s">
+        <v>312</v>
+      </c>
+      <c r="L43" s="67" t="s">
         <v>313</v>
-      </c>
-      <c r="L43" s="67" t="s">
-        <v>314</v>
       </c>
       <c r="M43" s="70"/>
       <c r="N43" s="70"/>
       <c r="O43" s="68"/>
-      <c r="P43" s="162"/>
-      <c r="Q43" s="162"/>
-      <c r="R43" s="162"/>
-      <c r="S43" s="162"/>
+      <c r="P43" s="167"/>
+      <c r="Q43" s="167"/>
+      <c r="R43" s="167"/>
+      <c r="S43" s="167"/>
     </row>
     <row r="44">
       <c r="A44" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="140" t="s">
         <v>315</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>316</v>
       </c>
       <c r="C44" s="92" t="s">
         <v>193</v>
@@ -5434,32 +5446,32 @@
       <c r="F44" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G44" s="165" t="s">
-        <v>317</v>
-      </c>
-      <c r="H44" s="138"/>
+      <c r="G44" s="170" t="s">
+        <v>316</v>
+      </c>
+      <c r="H44" s="139"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
-      <c r="K44" s="147">
+      <c r="K44" s="150">
         <v>0.0</v>
       </c>
-      <c r="L44" s="166" t="s">
+      <c r="L44" s="171" t="s">
         <v>67</v>
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
       <c r="O44" s="22"/>
-      <c r="P44" s="167"/>
-      <c r="Q44" s="167"/>
-      <c r="R44" s="167"/>
-      <c r="S44" s="167"/>
+      <c r="P44" s="172"/>
+      <c r="Q44" s="172"/>
+      <c r="R44" s="172"/>
+      <c r="S44" s="172"/>
     </row>
     <row r="45">
       <c r="A45" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="B45" s="140" t="s">
         <v>318</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>319</v>
       </c>
       <c r="C45" s="92" t="s">
         <v>198</v>
@@ -5471,25 +5483,25 @@
       <c r="F45" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="G45" s="165" t="s">
-        <v>320</v>
-      </c>
-      <c r="H45" s="138"/>
+      <c r="G45" s="170" t="s">
+        <v>319</v>
+      </c>
+      <c r="H45" s="139"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
-      <c r="K45" s="147" t="s">
+      <c r="K45" s="150" t="s">
+        <v>320</v>
+      </c>
+      <c r="L45" s="171" t="s">
         <v>321</v>
-      </c>
-      <c r="L45" s="166" t="s">
-        <v>322</v>
       </c>
       <c r="M45" s="20"/>
       <c r="N45" s="20"/>
       <c r="O45" s="22"/>
-      <c r="P45" s="167"/>
-      <c r="Q45" s="167"/>
-      <c r="R45" s="167"/>
-      <c r="S45" s="167"/>
+      <c r="P45" s="172"/>
+      <c r="Q45" s="172"/>
+      <c r="R45" s="172"/>
+      <c r="S45" s="172"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>
@@ -5517,236 +5529,236 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="168" t="s">
-        <v>323</v>
-      </c>
-      <c r="B1" s="169" t="s">
+      <c r="A1" s="173" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="169" t="s">
+      <c r="C1" s="174" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="170" t="s">
+      <c r="E1" s="175" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="59" t="s">
         <v>324</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="G1" s="175"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="176" t="s">
         <v>325</v>
       </c>
-      <c r="G1" s="170"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="171" t="s">
+      <c r="B2" s="177" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="172" t="s">
+      <c r="C2" s="178" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="173" t="s">
+      <c r="D2" s="168" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="163" t="s">
+      <c r="E2" s="177" t="s">
         <v>329</v>
-      </c>
-      <c r="E2" s="172" t="s">
-        <v>330</v>
       </c>
       <c r="F2" s="70"/>
       <c r="G2" s="70"/>
     </row>
     <row r="3">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="179" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="180" t="s">
         <v>331</v>
       </c>
-      <c r="B3" s="175" t="s">
+      <c r="C3" s="181" t="s">
         <v>332</v>
       </c>
-      <c r="C3" s="176" t="s">
-        <v>333</v>
-      </c>
-      <c r="D3" s="173"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="70"/>
       <c r="F3" s="70"/>
       <c r="G3" s="70"/>
     </row>
     <row r="4">
-      <c r="A4" s="177"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="179"/>
+      <c r="A4" s="182"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="184"/>
       <c r="E4" s="54"/>
       <c r="F4" s="54"/>
       <c r="G4" s="54"/>
     </row>
     <row r="5">
-      <c r="A5" s="180"/>
-      <c r="B5" s="180"/>
-      <c r="C5" s="181"/>
-      <c r="D5" s="182"/>
+      <c r="A5" s="185"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="187"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
     <row r="6">
-      <c r="A6" s="180"/>
-      <c r="B6" s="180"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="182"/>
+      <c r="A6" s="185"/>
+      <c r="B6" s="185"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="187"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
     </row>
     <row r="7">
-      <c r="A7" s="180"/>
-      <c r="B7" s="180"/>
-      <c r="C7" s="181"/>
-      <c r="D7" s="182"/>
+      <c r="A7" s="185"/>
+      <c r="B7" s="185"/>
+      <c r="C7" s="186"/>
+      <c r="D7" s="187"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
     </row>
     <row r="8">
-      <c r="A8" s="180"/>
-      <c r="B8" s="180"/>
-      <c r="C8" s="181"/>
-      <c r="D8" s="182"/>
+      <c r="A8" s="185"/>
+      <c r="B8" s="185"/>
+      <c r="C8" s="186"/>
+      <c r="D8" s="187"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
     <row r="9">
-      <c r="A9" s="180"/>
-      <c r="B9" s="180"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="182"/>
+      <c r="A9" s="185"/>
+      <c r="B9" s="185"/>
+      <c r="C9" s="186"/>
+      <c r="D9" s="187"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10">
-      <c r="A10" s="180"/>
-      <c r="B10" s="180"/>
-      <c r="C10" s="181"/>
-      <c r="D10" s="182"/>
+      <c r="A10" s="185"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="186"/>
+      <c r="D10" s="187"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
     <row r="11">
-      <c r="A11" s="180"/>
-      <c r="B11" s="180"/>
-      <c r="C11" s="181"/>
-      <c r="D11" s="182"/>
+      <c r="A11" s="185"/>
+      <c r="B11" s="185"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="187"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12">
-      <c r="A12" s="180"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="181"/>
-      <c r="D12" s="182"/>
+      <c r="A12" s="185"/>
+      <c r="B12" s="185"/>
+      <c r="C12" s="186"/>
+      <c r="D12" s="187"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13">
-      <c r="A13" s="180"/>
-      <c r="B13" s="180"/>
-      <c r="C13" s="181"/>
-      <c r="D13" s="182"/>
+      <c r="A13" s="185"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="186"/>
+      <c r="D13" s="187"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
     </row>
     <row r="14">
-      <c r="A14" s="180"/>
-      <c r="B14" s="180"/>
-      <c r="C14" s="181"/>
-      <c r="D14" s="182"/>
+      <c r="A14" s="185"/>
+      <c r="B14" s="185"/>
+      <c r="C14" s="186"/>
+      <c r="D14" s="187"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
     </row>
     <row r="15">
-      <c r="A15" s="180"/>
-      <c r="B15" s="180"/>
-      <c r="C15" s="181"/>
-      <c r="D15" s="182"/>
+      <c r="A15" s="185"/>
+      <c r="B15" s="185"/>
+      <c r="C15" s="186"/>
+      <c r="D15" s="187"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
     </row>
     <row r="16">
-      <c r="A16" s="180"/>
-      <c r="B16" s="180"/>
-      <c r="C16" s="181"/>
-      <c r="D16" s="182"/>
+      <c r="A16" s="185"/>
+      <c r="B16" s="185"/>
+      <c r="C16" s="186"/>
+      <c r="D16" s="187"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
     </row>
     <row r="17">
-      <c r="A17" s="180"/>
-      <c r="B17" s="180"/>
-      <c r="C17" s="181"/>
-      <c r="D17" s="182"/>
+      <c r="A17" s="185"/>
+      <c r="B17" s="185"/>
+      <c r="C17" s="186"/>
+      <c r="D17" s="187"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
     </row>
     <row r="18">
-      <c r="A18" s="180"/>
-      <c r="B18" s="180"/>
-      <c r="C18" s="181"/>
-      <c r="D18" s="182"/>
+      <c r="A18" s="185"/>
+      <c r="B18" s="185"/>
+      <c r="C18" s="186"/>
+      <c r="D18" s="187"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
     </row>
     <row r="19">
-      <c r="A19" s="180"/>
-      <c r="B19" s="180"/>
-      <c r="C19" s="181"/>
-      <c r="D19" s="182"/>
+      <c r="A19" s="185"/>
+      <c r="B19" s="185"/>
+      <c r="C19" s="186"/>
+      <c r="D19" s="187"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
     </row>
     <row r="20">
-      <c r="A20" s="180"/>
-      <c r="B20" s="180"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="182"/>
+      <c r="A20" s="185"/>
+      <c r="B20" s="185"/>
+      <c r="C20" s="186"/>
+      <c r="D20" s="187"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
     </row>
     <row r="21">
-      <c r="A21" s="180"/>
-      <c r="B21" s="180"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="182"/>
+      <c r="A21" s="185"/>
+      <c r="B21" s="185"/>
+      <c r="C21" s="186"/>
+      <c r="D21" s="187"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
     </row>
     <row r="22">
-      <c r="A22" s="180"/>
-      <c r="B22" s="180"/>
-      <c r="C22" s="181"/>
-      <c r="D22" s="182"/>
+      <c r="A22" s="185"/>
+      <c r="B22" s="185"/>
+      <c r="C22" s="186"/>
+      <c r="D22" s="187"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
     </row>
     <row r="23">
-      <c r="A23" s="180"/>
-      <c r="B23" s="180"/>
-      <c r="C23" s="181"/>
-      <c r="D23" s="182"/>
+      <c r="A23" s="185"/>
+      <c r="B23" s="185"/>
+      <c r="C23" s="186"/>
+      <c r="D23" s="187"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -5779,25 +5791,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="188" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="183" t="s">
+      <c r="C1" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="183" t="s">
+      <c r="D1" s="188" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G1" s="183" t="s">
+      <c r="G1" s="188" t="s">
         <v>95</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -5807,7 +5819,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" ht="73.5" customHeight="1">
@@ -5815,17 +5827,17 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C2" s="184"/>
+        <v>337</v>
+      </c>
+      <c r="C2" s="189"/>
       <c r="D2" s="64"/>
       <c r="E2" s="2"/>
-      <c r="G2" s="185"/>
+      <c r="G2" s="190"/>
       <c r="I2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="J2" s="191" t="s">
         <v>339</v>
-      </c>
-      <c r="J2" s="186" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="3" ht="73.5" customHeight="1">
@@ -5833,17 +5845,17 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C3" s="64"/>
       <c r="D3" s="64"/>
       <c r="E3" s="2"/>
-      <c r="G3" s="185"/>
+      <c r="G3" s="190"/>
       <c r="I3" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="4" ht="73.5" customHeight="1">
@@ -5851,14 +5863,14 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C4" s="64"/>
       <c r="D4" s="64"/>
       <c r="E4" s="2"/>
-      <c r="G4" s="185"/>
+      <c r="G4" s="190"/>
       <c r="I4" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -5867,17 +5879,17 @@
         <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
       <c r="E5" s="2"/>
-      <c r="G5" s="185"/>
+      <c r="G5" s="190"/>
       <c r="I5" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="6" ht="73.5" customHeight="1">
@@ -5885,46 +5897,46 @@
         <v>68</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C6" s="64"/>
       <c r="D6" s="64"/>
       <c r="E6" s="2"/>
-      <c r="G6" s="185"/>
+      <c r="G6" s="190"/>
       <c r="I6" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J6" s="116"/>
     </row>
     <row r="7" ht="73.5" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="192" t="s">
         <v>352</v>
-      </c>
-      <c r="C7" s="187" t="s">
-        <v>353</v>
       </c>
       <c r="D7" s="64"/>
       <c r="E7" s="2"/>
-      <c r="G7" s="185"/>
+      <c r="G7" s="190"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" ht="73.5" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="192"/>
+      <c r="D8" s="193" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="187"/>
-      <c r="D8" s="188" t="s">
-        <v>356</v>
-      </c>
       <c r="E8" s="2"/>
-      <c r="G8" s="185"/>
+      <c r="G8" s="190"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
@@ -5962,42 +5974,42 @@
         <v>8</v>
       </c>
       <c r="D1" s="58" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="194" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="64" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="189" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="64" t="s">
+      <c r="D2" s="194"/>
+      <c r="E2" s="64"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="194" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D2" s="189"/>
-      <c r="E2" s="64"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="189" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>361</v>
-      </c>
-      <c r="D3" s="189"/>
+      <c r="D3" s="194"/>
       <c r="E3" s="64"/>
       <c r="F3" s="98"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D4" s="54"/>
     </row>
@@ -6006,7 +6018,7 @@
         <v>180</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="54"/>
     </row>
@@ -6015,7 +6027,7 @@
         <v>187</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D6" s="54"/>
     </row>
@@ -6024,7 +6036,7 @@
         <v>200</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D7" s="54"/>
     </row>
@@ -6043,30 +6055,30 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.0"/>
+    <col customWidth="1" min="1" max="1" width="15.88"/>
     <col customWidth="1" min="3" max="3" width="33.38"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="195" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="196" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="191" t="s">
+      <c r="C2" s="197" t="s">
         <v>368</v>
-      </c>
-      <c r="C2" s="192" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -6094,16 +6106,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="4">
@@ -6111,20 +6123,20 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>